<commit_message>
Remove PII from tmplate
</commit_message>
<xml_diff>
--- a/MBP_Invoice_Template.xlsx
+++ b/MBP_Invoice_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Print" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t xml:space="preserve">Invoice</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Client:</t>
   </si>
   <si>
-    <t xml:space="preserve">Tax </t>
+    <t xml:space="preserve">Tax</t>
   </si>
   <si>
     <t xml:space="preserve">MBP:</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Grand Total</t>
   </si>
   <si>
-    <t xml:space="preserve">#02331</t>
+    <t xml:space="preserve">#02332</t>
   </si>
   <si>
     <t xml:space="preserve">Invoice Number</t>
@@ -88,9 +88,6 @@
     <t xml:space="preserve">Discount total</t>
   </si>
   <si>
-    <t xml:space="preserve">Eddie McDonald</t>
-  </si>
-  <si>
     <t xml:space="preserve">Issued To</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tax Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tax</t>
   </si>
   <si>
     <t xml:space="preserve">Incl. Sig?</t>
@@ -274,7 +268,7 @@
     <numFmt numFmtId="171" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="172" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -366,12 +360,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Ubuntu Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="ubuntu mono"/>
       <family val="0"/>
       <charset val="1"/>
@@ -549,6 +537,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -589,10 +581,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,6 +589,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -653,7 +645,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -673,7 +665,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,8 +677,8 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="171" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -705,10 +697,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -717,7 +705,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -853,10 +841,10 @@
       <xdr:rowOff>210600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>52920</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>545040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1890360</xdr:rowOff>
+      <xdr:rowOff>1889640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -870,7 +858,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12600" y="210600"/>
-          <a:ext cx="7418880" cy="1679760"/>
+          <a:ext cx="7418160" cy="1679040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -885,15 +873,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>712080</xdr:colOff>
+      <xdr:colOff>712440</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>54720</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>624240</xdr:rowOff>
+      <xdr:rowOff>623880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -906,8 +894,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5919480" y="7654680"/>
-          <a:ext cx="1130760" cy="530280"/>
+          <a:off x="5810040" y="7655040"/>
+          <a:ext cx="1130040" cy="529560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -922,15 +910,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>273960</xdr:colOff>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1306440</xdr:colOff>
+      <xdr:colOff>1306080</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -943,8 +931,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1823040" y="6826680"/>
-          <a:ext cx="1434600" cy="604440"/>
+          <a:off x="1713600" y="6827040"/>
+          <a:ext cx="1433880" cy="603720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -966,13 +954,13 @@
   </sheetPr>
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.7"/>
@@ -981,7 +969,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.43"/>
@@ -1008,7 +996,7 @@
       <c r="G3" s="4"/>
       <c r="I3" s="5" t="str">
         <f aca="false">Data!B3</f>
-        <v>#02331</v>
+        <v>#02332</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1042,16 +1030,16 @@
       <c r="A6" s="8"/>
       <c r="B6" s="12" t="n">
         <f aca="false">Data!B5</f>
-        <v>44801</v>
+        <v>0</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="4"/>
       <c r="F6" s="10"/>
       <c r="G6" s="4"/>
-      <c r="I6" s="11" t="str">
+      <c r="I6" s="11" t="n">
         <f aca="false">Data!B4</f>
-        <v>Eddie McDonald</v>
+        <v>0</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="4"/>
@@ -1108,20 +1096,20 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20" t="n">
+      <c r="F9" s="20"/>
+      <c r="G9" s="21" t="n">
         <f aca="false">Data!D21</f>
         <v>50</v>
       </c>
-      <c r="H9" s="20" t="n">
+      <c r="H9" s="21" t="n">
         <f aca="false">Data!C21</f>
         <v>1</v>
       </c>
-      <c r="I9" s="21" t="n">
+      <c r="I9" s="22" t="n">
         <f aca="false">Data!G21</f>
         <v>50</v>
       </c>
-      <c r="J9" s="21"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="17"/>
       <c r="L9" s="4"/>
     </row>
@@ -1131,26 +1119,26 @@
         <f aca="false">Data!B18</f>
         <v>5</v>
       </c>
-      <c r="C10" s="19" t="str">
+      <c r="C10" s="20" t="str">
         <f aca="false">Data!E18</f>
         <v>Domain Services</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20" t="n">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21" t="n">
         <f aca="false">Data!D18</f>
         <v>100</v>
       </c>
-      <c r="H10" s="20" t="n">
+      <c r="H10" s="21" t="n">
         <f aca="false">Data!C18</f>
         <v>0</v>
       </c>
-      <c r="I10" s="21" t="n">
+      <c r="I10" s="22" t="n">
         <f aca="false">Data!G18</f>
         <v>0</v>
       </c>
-      <c r="J10" s="21"/>
+      <c r="J10" s="22"/>
       <c r="K10" s="17"/>
       <c r="L10" s="4"/>
     </row>
@@ -1160,26 +1148,26 @@
         <f aca="false">Data!B19</f>
         <v>6</v>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="20" t="str">
         <f aca="false">Data!E19</f>
         <v>Email Setup</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20" t="n">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21" t="n">
         <f aca="false">Data!D19</f>
         <v>100</v>
       </c>
-      <c r="H11" s="20" t="n">
+      <c r="H11" s="21" t="n">
         <f aca="false">Data!C19</f>
         <v>0</v>
       </c>
-      <c r="I11" s="21" t="n">
+      <c r="I11" s="22" t="n">
         <f aca="false">Data!G19</f>
         <v>0</v>
       </c>
-      <c r="J11" s="21"/>
+      <c r="J11" s="22"/>
       <c r="K11" s="17"/>
       <c r="L11" s="4"/>
     </row>
@@ -1189,26 +1177,26 @@
         <f aca="false">Data!B22</f>
         <v>12</v>
       </c>
-      <c r="C12" s="19" t="str">
+      <c r="C12" s="20" t="str">
         <f aca="false">Data!E22</f>
         <v>Dynamic Pages</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20" t="n">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21" t="n">
         <f aca="false">Data!D22</f>
         <v>100</v>
       </c>
-      <c r="H12" s="20" t="n">
+      <c r="H12" s="21" t="n">
         <f aca="false">Data!C22</f>
         <v>2</v>
       </c>
-      <c r="I12" s="21" t="n">
+      <c r="I12" s="22" t="n">
         <f aca="false">Data!G22</f>
         <v>200</v>
       </c>
-      <c r="J12" s="21"/>
+      <c r="J12" s="22"/>
       <c r="K12" s="17"/>
       <c r="L12" s="4"/>
     </row>
@@ -1218,26 +1206,26 @@
         <f aca="false">Data!B15</f>
         <v>2</v>
       </c>
-      <c r="C13" s="22" t="str">
+      <c r="C13" s="23" t="str">
         <f aca="false">Data!E15</f>
         <v>Site Setup</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="20" t="n">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="21" t="n">
         <f aca="false">Data!D15</f>
         <v>100</v>
       </c>
-      <c r="H13" s="20" t="n">
+      <c r="H13" s="21" t="n">
         <f aca="false">Data!C15</f>
         <v>1</v>
       </c>
-      <c r="I13" s="21" t="n">
+      <c r="I13" s="22" t="n">
         <f aca="false">Data!G15</f>
         <v>100</v>
       </c>
-      <c r="J13" s="21"/>
+      <c r="J13" s="22"/>
       <c r="K13" s="17"/>
       <c r="L13" s="4"/>
     </row>
@@ -1247,26 +1235,26 @@
         <f aca="false">Data!B17</f>
         <v>4</v>
       </c>
-      <c r="C14" s="19" t="str">
+      <c r="C14" s="20" t="str">
         <f aca="false">Data!E17</f>
         <v>File Sanitation</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20" t="n">
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21" t="n">
         <f aca="false">Data!D17</f>
         <v>100</v>
       </c>
-      <c r="H14" s="20" t="n">
+      <c r="H14" s="21" t="n">
         <f aca="false">Data!C17</f>
         <v>0</v>
       </c>
-      <c r="I14" s="21" t="n">
+      <c r="I14" s="22" t="n">
         <f aca="false">Data!G17</f>
         <v>0</v>
       </c>
-      <c r="J14" s="21"/>
+      <c r="J14" s="22"/>
       <c r="K14" s="17"/>
       <c r="L14" s="4"/>
     </row>
@@ -1276,26 +1264,26 @@
         <f aca="false">Data!B14</f>
         <v>1</v>
       </c>
-      <c r="C15" s="22" t="str">
+      <c r="C15" s="23" t="str">
         <f aca="false">Data!E14</f>
         <v>Website hosting</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="20" t="n">
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="21" t="n">
         <f aca="false">Data!D14</f>
         <v>100</v>
       </c>
-      <c r="H15" s="20" t="n">
+      <c r="H15" s="21" t="n">
         <f aca="false">Data!C14</f>
         <v>0</v>
       </c>
-      <c r="I15" s="21" t="n">
+      <c r="I15" s="22" t="n">
         <f aca="false">Data!G14</f>
         <v>0</v>
       </c>
-      <c r="J15" s="21"/>
+      <c r="J15" s="22"/>
       <c r="K15" s="17"/>
       <c r="L15" s="4"/>
     </row>
@@ -1305,26 +1293,26 @@
         <f aca="false">Data!B16</f>
         <v>3</v>
       </c>
-      <c r="C16" s="19" t="str">
+      <c r="C16" s="20" t="str">
         <f aca="false">Data!E16</f>
         <v>File Structuring &gt;500</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20" t="n">
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21" t="n">
         <f aca="false">Data!D16</f>
         <v>100</v>
       </c>
-      <c r="H16" s="20" t="n">
+      <c r="H16" s="21" t="n">
         <f aca="false">Data!C16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="21" t="n">
+      <c r="I16" s="22" t="n">
         <f aca="false">Data!G16</f>
         <v>0</v>
       </c>
-      <c r="J16" s="21"/>
+      <c r="J16" s="22"/>
       <c r="K16" s="17"/>
       <c r="L16" s="4"/>
     </row>
@@ -1334,26 +1322,26 @@
         <f aca="false">Data!B20</f>
         <v>7</v>
       </c>
-      <c r="C17" s="19" t="str">
+      <c r="C17" s="20" t="str">
         <f aca="false">Data!E20</f>
         <v>CDN Setup</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20" t="n">
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21" t="n">
         <f aca="false">Data!D20</f>
         <v>100</v>
       </c>
-      <c r="H17" s="20" t="n">
+      <c r="H17" s="21" t="n">
         <f aca="false">Data!C20</f>
         <v>0</v>
       </c>
-      <c r="I17" s="21" t="n">
+      <c r="I17" s="22" t="n">
         <f aca="false">Data!G20</f>
         <v>0</v>
       </c>
-      <c r="J17" s="21"/>
+      <c r="J17" s="22"/>
       <c r="K17" s="17"/>
       <c r="L17" s="4"/>
     </row>
@@ -1363,26 +1351,26 @@
         <f aca="false">Data!B23</f>
         <v>13</v>
       </c>
-      <c r="C18" s="19" t="str">
+      <c r="C18" s="20" t="str">
         <f aca="false">Data!E23</f>
         <v>Custom Feed</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20" t="n">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21" t="n">
         <f aca="false">Data!D23</f>
         <v>100</v>
       </c>
-      <c r="H18" s="20" t="n">
+      <c r="H18" s="21" t="n">
         <f aca="false">Data!C23</f>
         <v>2</v>
       </c>
-      <c r="I18" s="21" t="n">
+      <c r="I18" s="22" t="n">
         <f aca="false">Data!G23</f>
         <v>200</v>
       </c>
-      <c r="J18" s="21"/>
+      <c r="J18" s="22"/>
       <c r="K18" s="17"/>
       <c r="L18" s="4"/>
     </row>
@@ -1392,26 +1380,26 @@
         <f aca="false">Data!B24</f>
         <v>14</v>
       </c>
-      <c r="C19" s="19" t="str">
+      <c r="C19" s="20" t="str">
         <f aca="false">Data!E24</f>
         <v>Custom Frontend Components</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20" t="n">
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21" t="n">
         <f aca="false">Data!D24</f>
         <v>100</v>
       </c>
-      <c r="H19" s="20" t="n">
+      <c r="H19" s="21" t="n">
         <f aca="false">Data!C24</f>
         <v>0</v>
       </c>
-      <c r="I19" s="21" t="n">
+      <c r="I19" s="22" t="n">
         <f aca="false">Data!G24</f>
         <v>0</v>
       </c>
-      <c r="J19" s="21"/>
+      <c r="J19" s="22"/>
       <c r="K19" s="17"/>
       <c r="L19" s="4"/>
     </row>
@@ -1421,26 +1409,26 @@
         <f aca="false">Data!B25</f>
         <v>15</v>
       </c>
-      <c r="C20" s="19" t="str">
+      <c r="C20" s="20" t="str">
         <f aca="false">Data!E25</f>
         <v>Custom Backend Components</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20" t="n">
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21" t="n">
         <f aca="false">Data!D25</f>
         <v>150</v>
       </c>
-      <c r="H20" s="20" t="n">
+      <c r="H20" s="21" t="n">
         <f aca="false">Data!C25</f>
         <v>0</v>
       </c>
-      <c r="I20" s="21" t="n">
+      <c r="I20" s="22" t="n">
         <f aca="false">Data!G25</f>
         <v>0</v>
       </c>
-      <c r="J20" s="21"/>
+      <c r="J20" s="22"/>
       <c r="K20" s="17"/>
       <c r="L20" s="4"/>
     </row>
@@ -1450,26 +1438,26 @@
         <f aca="false">Data!B26</f>
         <v>51</v>
       </c>
-      <c r="C21" s="19" t="str">
+      <c r="C21" s="20" t="str">
         <f aca="false">Data!E26</f>
         <v>Site Migration &gt;50 Pages</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20" t="n">
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21" t="n">
         <f aca="false">Data!D26</f>
         <v>300</v>
       </c>
-      <c r="H21" s="20" t="n">
+      <c r="H21" s="21" t="n">
         <f aca="false">Data!C26</f>
         <v>0</v>
       </c>
-      <c r="I21" s="21" t="n">
+      <c r="I21" s="22" t="n">
         <f aca="false">Data!G26</f>
         <v>0</v>
       </c>
-      <c r="J21" s="21"/>
+      <c r="J21" s="22"/>
       <c r="K21" s="17"/>
       <c r="L21" s="4"/>
     </row>
@@ -1479,26 +1467,26 @@
         <f aca="false">Data!B27</f>
         <v>52</v>
       </c>
-      <c r="C22" s="22" t="str">
+      <c r="C22" s="23" t="str">
         <f aca="false">Data!E27</f>
         <v>Site Migration &gt;100&lt;50 Pages</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="20" t="n">
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="21" t="n">
         <f aca="false">Data!D27</f>
         <v>600</v>
       </c>
-      <c r="H22" s="20" t="n">
+      <c r="H22" s="21" t="n">
         <f aca="false">Data!C27</f>
         <v>0</v>
       </c>
-      <c r="I22" s="21" t="n">
+      <c r="I22" s="22" t="n">
         <f aca="false">Data!G27</f>
         <v>0</v>
       </c>
-      <c r="J22" s="21"/>
+      <c r="J22" s="22"/>
       <c r="K22" s="17"/>
       <c r="L22" s="4"/>
     </row>
@@ -1508,26 +1496,26 @@
         <f aca="false">Data!B28</f>
         <v>101</v>
       </c>
-      <c r="C23" s="22" t="str">
+      <c r="C23" s="23" t="str">
         <f aca="false">Data!E28</f>
         <v>Storefront – Woocommerce</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="20" t="n">
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="21" t="n">
         <f aca="false">Data!D28</f>
         <v>450</v>
       </c>
-      <c r="H23" s="20" t="n">
+      <c r="H23" s="21" t="n">
         <f aca="false">Data!C28</f>
         <v>1</v>
       </c>
-      <c r="I23" s="21" t="n">
+      <c r="I23" s="22" t="n">
         <f aca="false">Data!G28</f>
         <v>450</v>
       </c>
-      <c r="J23" s="21"/>
+      <c r="J23" s="22"/>
       <c r="K23" s="17"/>
       <c r="L23" s="4"/>
     </row>
@@ -1537,26 +1525,26 @@
         <f aca="false">Data!B32</f>
         <v>503</v>
       </c>
-      <c r="C24" s="19" t="str">
+      <c r="C24" s="20" t="str">
         <f aca="false">Data!E32</f>
         <v>Logo Rework</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="20" t="n">
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21" t="n">
         <f aca="false">Data!D32</f>
         <v>200</v>
       </c>
-      <c r="H24" s="20" t="n">
+      <c r="H24" s="21" t="n">
         <f aca="false">Data!C32</f>
         <v>0</v>
       </c>
-      <c r="I24" s="21" t="n">
+      <c r="I24" s="22" t="n">
         <f aca="false">Data!G32</f>
         <v>0</v>
       </c>
-      <c r="J24" s="21"/>
+      <c r="J24" s="22"/>
       <c r="K24" s="17"/>
       <c r="L24" s="4"/>
     </row>
@@ -1566,26 +1554,26 @@
         <f aca="false">Data!B33</f>
         <v>504</v>
       </c>
-      <c r="C25" s="19" t="str">
+      <c r="C25" s="20" t="str">
         <f aca="false">Data!E33</f>
         <v>Brand Organization</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20" t="n">
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21" t="n">
         <f aca="false">Data!D33</f>
         <v>300</v>
       </c>
-      <c r="H25" s="20" t="n">
+      <c r="H25" s="21" t="n">
         <f aca="false">Data!C33</f>
         <v>0</v>
       </c>
-      <c r="I25" s="21" t="n">
+      <c r="I25" s="22" t="n">
         <f aca="false">Data!G33</f>
         <v>0</v>
       </c>
-      <c r="J25" s="21"/>
+      <c r="J25" s="22"/>
       <c r="K25" s="17"/>
       <c r="L25" s="4"/>
     </row>
@@ -1595,26 +1583,26 @@
         <f aca="false">Data!B34</f>
         <v>505</v>
       </c>
-      <c r="C26" s="19" t="str">
+      <c r="C26" s="20" t="str">
         <f aca="false">Data!E34</f>
         <v>Copywriting</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="20" t="n">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21" t="n">
         <f aca="false">Data!D34</f>
         <v>50</v>
       </c>
-      <c r="H26" s="20" t="n">
+      <c r="H26" s="21" t="n">
         <f aca="false">Data!C34</f>
         <v>0</v>
       </c>
-      <c r="I26" s="21" t="n">
+      <c r="I26" s="22" t="n">
         <f aca="false">Data!G34</f>
         <v>0</v>
       </c>
-      <c r="J26" s="21"/>
+      <c r="J26" s="22"/>
       <c r="K26" s="17"/>
       <c r="L26" s="4"/>
     </row>
@@ -1624,26 +1612,26 @@
         <f aca="false">Data!B35</f>
         <v>1000</v>
       </c>
-      <c r="C27" s="19" t="str">
+      <c r="C27" s="20" t="str">
         <f aca="false">Data!E35</f>
         <v>General Contracting</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20" t="n">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21" t="n">
         <f aca="false">Data!D35</f>
         <v>100</v>
       </c>
-      <c r="H27" s="20" t="n">
+      <c r="H27" s="21" t="n">
         <f aca="false">Data!C35</f>
         <v>0</v>
       </c>
-      <c r="I27" s="21" t="n">
+      <c r="I27" s="22" t="n">
         <f aca="false">Data!G35</f>
         <v>0</v>
       </c>
-      <c r="J27" s="21"/>
+      <c r="J27" s="22"/>
       <c r="K27" s="17"/>
       <c r="L27" s="4"/>
     </row>
@@ -1653,26 +1641,26 @@
         <f aca="false">Data!B36</f>
         <v>1001</v>
       </c>
-      <c r="C28" s="19" t="str">
+      <c r="C28" s="20" t="str">
         <f aca="false">Data!E36</f>
         <v>Web Consultation</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="20" t="n">
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21" t="n">
         <f aca="false">Data!D36</f>
         <v>100</v>
       </c>
-      <c r="H28" s="20" t="n">
+      <c r="H28" s="21" t="n">
         <f aca="false">Data!C36</f>
         <v>0</v>
       </c>
-      <c r="I28" s="21" t="n">
+      <c r="I28" s="22" t="n">
         <f aca="false">Data!G36</f>
         <v>0</v>
       </c>
-      <c r="J28" s="21"/>
+      <c r="J28" s="22"/>
       <c r="K28" s="17"/>
       <c r="L28" s="4"/>
     </row>
@@ -1682,26 +1670,26 @@
         <f aca="false">Data!B39</f>
         <v>1004</v>
       </c>
-      <c r="C29" s="19" t="str">
+      <c r="C29" s="20" t="str">
         <f aca="false">Data!E39</f>
         <v>Sales Consultation</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="20" t="n">
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21" t="n">
         <f aca="false">Data!D39</f>
         <v>100</v>
       </c>
-      <c r="H29" s="20" t="n">
+      <c r="H29" s="21" t="n">
         <f aca="false">Data!C39</f>
         <v>0</v>
       </c>
-      <c r="I29" s="21" t="n">
+      <c r="I29" s="22" t="n">
         <f aca="false">Data!G39</f>
         <v>0</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="22"/>
       <c r="K29" s="17"/>
       <c r="L29" s="4"/>
     </row>
@@ -1711,40 +1699,40 @@
         <f aca="false">Data!B40</f>
         <v>0</v>
       </c>
-      <c r="C30" s="19" t="n">
+      <c r="C30" s="20" t="n">
         <f aca="false">Data!E40</f>
         <v>0</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="20" t="n">
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21" t="n">
         <f aca="false">Data!D40</f>
         <v>0</v>
       </c>
-      <c r="H30" s="20" t="n">
+      <c r="H30" s="21" t="n">
         <f aca="false">Data!C40</f>
         <v>0</v>
       </c>
-      <c r="I30" s="21" t="n">
+      <c r="I30" s="22" t="n">
         <f aca="false">Data!G40</f>
         <v>0</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="22"/>
       <c r="K30" s="17"/>
       <c r="L30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="17"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="28"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="29"/>
       <c r="K31" s="17"/>
       <c r="L31" s="4"/>
     </row>
@@ -1770,10 +1758,10 @@
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
-      <c r="H33" s="31" t="s">
+      <c r="H33" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="32" t="n">
+      <c r="I33" s="33" t="n">
         <f aca="false">Data!F7</f>
         <v>1000</v>
       </c>
@@ -1789,10 +1777,10 @@
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="33" t="s">
+      <c r="H34" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="32" t="n">
+      <c r="I34" s="33" t="n">
         <f aca="false">Data!G4</f>
         <v>550</v>
       </c>
@@ -1802,21 +1790,21 @@
     </row>
     <row r="35" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="17"/>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
       <c r="F35" s="17"/>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I35" s="32" t="n">
+      <c r="I35" s="33" t="n">
         <f aca="false">Data!G7</f>
-        <v>450</v>
-      </c>
-      <c r="J35" s="36"/>
+        <v>200</v>
+      </c>
+      <c r="J35" s="37"/>
       <c r="K35" s="17"/>
       <c r="L35" s="4"/>
     </row>
@@ -1827,34 +1815,34 @@
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="17"/>
-      <c r="H36" s="33" t="s">
+      <c r="H36" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="32" t="n">
+      <c r="I36" s="33" t="n">
         <f aca="false">Data!F8</f>
         <v>29.25</v>
       </c>
-      <c r="J36" s="37"/>
+      <c r="J36" s="38"/>
       <c r="K36" s="17"/>
       <c r="L36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="17"/>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="17"/>
-      <c r="H37" s="33" t="s">
+      <c r="H37" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I37" s="32" t="n">
+      <c r="I37" s="33" t="n">
         <f aca="false">Data!F3</f>
-        <v>0</v>
-      </c>
-      <c r="J37" s="37"/>
+        <v>250</v>
+      </c>
+      <c r="J37" s="38"/>
       <c r="K37" s="17"/>
       <c r="L37" s="4"/>
     </row>
@@ -1864,15 +1852,15 @@
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34" t="s">
+      <c r="G38" s="35"/>
+      <c r="H38" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I38" s="40" t="n">
+      <c r="I38" s="41" t="n">
         <f aca="false">Data!F10</f>
-        <v>479.25</v>
-      </c>
-      <c r="J38" s="36"/>
+        <v>229.25</v>
+      </c>
+      <c r="J38" s="37"/>
       <c r="K38" s="17"/>
       <c r="L38" s="4"/>
     </row>
@@ -1911,7 +1899,7 @@
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="11"/>
-      <c r="F42" s="23"/>
+      <c r="F42" s="24"/>
       <c r="K42" s="10"/>
       <c r="L42" s="4"/>
     </row>
@@ -1998,8 +1986,8 @@
   </sheetPr>
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2015,247 +2003,245 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42" t="s">
+      <c r="A3" s="42"/>
+      <c r="B3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="43" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="45" t="s">
+      <c r="F3" s="45" t="n">
+        <v>250</v>
+      </c>
+      <c r="G3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
     </row>
     <row r="4" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="46"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="47"/>
+      <c r="C4" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="43" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="44" t="n">
+      <c r="F4" s="45" t="n">
         <v>50</v>
       </c>
-      <c r="G4" s="47" t="n">
+      <c r="G4" s="48" t="n">
         <f aca="false">IF(F5="Y",(PRODUCT(F7,0.5)+F4),F4)</f>
         <v>550</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
     </row>
     <row r="5" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="46"/>
-      <c r="B5" s="48" t="n">
-        <v>44801</v>
-      </c>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="43" t="s">
+      <c r="F5" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="G5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="H5" s="51"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+    </row>
+    <row r="6" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="47"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-    </row>
-    <row r="6" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="51" t="n">
+      <c r="F6" s="52" t="n">
         <v>0.065</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
     </row>
     <row r="7" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="43" t="s">
+      <c r="A7" s="47"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="52" t="n">
+      <c r="F7" s="53" t="n">
         <f aca="false">SUM(G14:G40)</f>
         <v>1000</v>
       </c>
-      <c r="G7" s="47" t="n">
+      <c r="G7" s="48" t="n">
+        <f aca="false">IF(F5="Y",(PRODUCT(F7,0.5)-F4)-F3,F7-F4-F3)</f>
+        <v>200</v>
+      </c>
+      <c r="H7" s="48"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+    </row>
+    <row r="8" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="53" t="n">
+        <f aca="false">(G8*F6)</f>
+        <v>29.25</v>
+      </c>
+      <c r="G8" s="54" t="n">
         <f aca="false">IF(F5="Y",(PRODUCT(F7,0.5)-F4),F7-F4)</f>
         <v>450</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="52" t="n">
-        <f aca="false">(G7*F6)</f>
-        <v>29.25</v>
-      </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
     </row>
     <row r="9" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="46"/>
-      <c r="B9" s="54" t="n">
+      <c r="A9" s="47"/>
+      <c r="B9" s="55" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
     </row>
     <row r="10" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="46"/>
-      <c r="B10" s="54" t="n">
+      <c r="A10" s="47"/>
+      <c r="B10" s="55" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="57" t="n">
+        <f aca="false">IF(F9="N",G7+F8,G7)</f>
+        <v>229.25</v>
+      </c>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="42"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="42"/>
+      <c r="B13" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="56" t="n">
-        <f aca="false">IF(F9="N",G7+F8,G7)</f>
-        <v>479.25</v>
-      </c>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41"/>
-      <c r="B13" s="43" t="s">
+      <c r="D13" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="E13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="F13" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="G13" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41"/>
-      <c r="B14" s="57" t="n">
+      <c r="A14" s="42"/>
+      <c r="B14" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A2</f>
         <v>1</v>
       </c>
-      <c r="C14" s="58" t="n">
+      <c r="C14" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="59" t="n">
@@ -2279,12 +2265,12 @@
       <c r="J14" s="62"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41"/>
-      <c r="B15" s="57" t="n">
+      <c r="A15" s="42"/>
+      <c r="B15" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A3</f>
         <v>2</v>
       </c>
-      <c r="C15" s="58" t="n">
+      <c r="C15" s="52" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="59" t="n">
@@ -2308,12 +2294,12 @@
       <c r="J15" s="62"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41"/>
-      <c r="B16" s="57" t="n">
+      <c r="A16" s="42"/>
+      <c r="B16" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A4</f>
         <v>3</v>
       </c>
-      <c r="C16" s="58" t="n">
+      <c r="C16" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="59" t="n">
@@ -2337,12 +2323,12 @@
       <c r="J16" s="62"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41"/>
-      <c r="B17" s="57" t="n">
+      <c r="A17" s="42"/>
+      <c r="B17" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A5</f>
         <v>4</v>
       </c>
-      <c r="C17" s="58" t="n">
+      <c r="C17" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="59" t="n">
@@ -2361,17 +2347,17 @@
         <f aca="false">PRODUCT(C17,D17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41"/>
-      <c r="B18" s="57" t="n">
+      <c r="A18" s="42"/>
+      <c r="B18" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A6</f>
         <v>5</v>
       </c>
-      <c r="C18" s="58" t="n">
+      <c r="C18" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="59" t="n">
@@ -2390,17 +2376,17 @@
         <f aca="false">PRODUCT(C18,D18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41"/>
-      <c r="B19" s="57" t="n">
+      <c r="A19" s="42"/>
+      <c r="B19" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A7</f>
         <v>6</v>
       </c>
-      <c r="C19" s="58" t="n">
+      <c r="C19" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D19" s="59" t="n">
@@ -2419,17 +2405,17 @@
         <f aca="false">PRODUCT(C19,D19)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41"/>
-      <c r="B20" s="57" t="n">
+      <c r="A20" s="42"/>
+      <c r="B20" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A8</f>
         <v>7</v>
       </c>
-      <c r="C20" s="58" t="n">
+      <c r="C20" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="59" t="n">
@@ -2448,17 +2434,17 @@
         <f aca="false">PRODUCT(C20,D20)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41"/>
-      <c r="B21" s="57" t="n">
+      <c r="A21" s="42"/>
+      <c r="B21" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A9</f>
         <v>11</v>
       </c>
-      <c r="C21" s="58" t="n">
+      <c r="C21" s="52" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="59" t="n">
@@ -2477,17 +2463,17 @@
         <f aca="false">PRODUCT(C21,D21)</f>
         <v>50</v>
       </c>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41"/>
-      <c r="B22" s="57" t="n">
+      <c r="A22" s="42"/>
+      <c r="B22" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A10</f>
         <v>12</v>
       </c>
-      <c r="C22" s="58" t="n">
+      <c r="C22" s="52" t="n">
         <v>2</v>
       </c>
       <c r="D22" s="59" t="n">
@@ -2506,17 +2492,17 @@
         <f aca="false">PRODUCT(C22,D22)</f>
         <v>200</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41"/>
-      <c r="B23" s="57" t="n">
+      <c r="A23" s="42"/>
+      <c r="B23" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A11</f>
         <v>13</v>
       </c>
-      <c r="C23" s="58" t="n">
+      <c r="C23" s="52" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="59" t="n">
@@ -2535,17 +2521,17 @@
         <f aca="false">PRODUCT(C23,D23)</f>
         <v>200</v>
       </c>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41"/>
-      <c r="B24" s="57" t="n">
+      <c r="A24" s="42"/>
+      <c r="B24" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A12</f>
         <v>14</v>
       </c>
-      <c r="C24" s="58" t="n">
+      <c r="C24" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D24" s="59" t="n">
@@ -2564,17 +2550,17 @@
         <f aca="false">PRODUCT(C24,D24)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41"/>
-      <c r="B25" s="57" t="n">
+      <c r="A25" s="42"/>
+      <c r="B25" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A13</f>
         <v>15</v>
       </c>
-      <c r="C25" s="58" t="n">
+      <c r="C25" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D25" s="59" t="n">
@@ -2593,17 +2579,17 @@
         <f aca="false">PRODUCT(C25,D25)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41"/>
-      <c r="B26" s="57" t="n">
+      <c r="A26" s="42"/>
+      <c r="B26" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A14</f>
         <v>51</v>
       </c>
-      <c r="C26" s="58" t="n">
+      <c r="C26" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D26" s="59" t="n">
@@ -2622,17 +2608,17 @@
         <f aca="false">PRODUCT(C26,D26)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41"/>
-      <c r="B27" s="57" t="n">
+      <c r="A27" s="42"/>
+      <c r="B27" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A15</f>
         <v>52</v>
       </c>
-      <c r="C27" s="58" t="n">
+      <c r="C27" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D27" s="59" t="n">
@@ -2651,17 +2637,17 @@
         <f aca="false">PRODUCT(C27,D27)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="41"/>
-      <c r="B28" s="57" t="n">
+      <c r="A28" s="42"/>
+      <c r="B28" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A16</f>
         <v>101</v>
       </c>
-      <c r="C28" s="58" t="n">
+      <c r="C28" s="52" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="59" t="n">
@@ -2680,17 +2666,17 @@
         <f aca="false">PRODUCT(C28,D28)</f>
         <v>450</v>
       </c>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="41"/>
-      <c r="B29" s="57" t="n">
+      <c r="A29" s="42"/>
+      <c r="B29" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A17</f>
         <v>500</v>
       </c>
-      <c r="C29" s="58" t="n">
+      <c r="C29" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="59" t="n">
@@ -2709,17 +2695,17 @@
         <f aca="false">PRODUCT(C29,D29)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="41"/>
-      <c r="B30" s="57" t="n">
+      <c r="A30" s="42"/>
+      <c r="B30" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A18</f>
         <v>501</v>
       </c>
-      <c r="C30" s="58" t="n">
+      <c r="C30" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D30" s="59" t="n">
@@ -2738,17 +2724,17 @@
         <f aca="false">PRODUCT(C30,D30)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="41"/>
-      <c r="B31" s="57" t="n">
+      <c r="A31" s="42"/>
+      <c r="B31" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A19</f>
         <v>502</v>
       </c>
-      <c r="C31" s="58" t="n">
+      <c r="C31" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D31" s="59" t="n">
@@ -2767,17 +2753,17 @@
         <f aca="false">PRODUCT(C31,D31)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="41"/>
-      <c r="B32" s="57" t="n">
+      <c r="A32" s="42"/>
+      <c r="B32" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A20</f>
         <v>503</v>
       </c>
-      <c r="C32" s="58" t="n">
+      <c r="C32" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D32" s="59" t="n">
@@ -2796,17 +2782,17 @@
         <f aca="false">PRODUCT(C32,D32)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="41"/>
-      <c r="B33" s="57" t="n">
+      <c r="A33" s="42"/>
+      <c r="B33" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A21</f>
         <v>504</v>
       </c>
-      <c r="C33" s="58" t="n">
+      <c r="C33" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D33" s="59" t="n">
@@ -2825,17 +2811,17 @@
         <f aca="false">PRODUCT(C33,D33)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="41"/>
-      <c r="B34" s="57" t="n">
+      <c r="A34" s="42"/>
+      <c r="B34" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A22</f>
         <v>505</v>
       </c>
-      <c r="C34" s="58" t="n">
+      <c r="C34" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D34" s="59" t="n">
@@ -2854,17 +2840,17 @@
         <f aca="false">PRODUCT(C34,D34)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="41"/>
-      <c r="B35" s="57" t="n">
+      <c r="A35" s="42"/>
+      <c r="B35" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A23</f>
         <v>1000</v>
       </c>
-      <c r="C35" s="58" t="n">
+      <c r="C35" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="59" t="n">
@@ -2883,17 +2869,17 @@
         <f aca="false">PRODUCT(C35,D35)</f>
         <v>0</v>
       </c>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="41"/>
-      <c r="B36" s="57" t="n">
+      <c r="A36" s="42"/>
+      <c r="B36" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A24</f>
         <v>1001</v>
       </c>
-      <c r="C36" s="58" t="n">
+      <c r="C36" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D36" s="59" t="n">
@@ -2912,17 +2898,17 @@
         <f aca="false">PRODUCT(C36,D36)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="41"/>
-      <c r="B37" s="57" t="n">
+      <c r="A37" s="42"/>
+      <c r="B37" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A25</f>
         <v>1002</v>
       </c>
-      <c r="C37" s="58" t="n">
+      <c r="C37" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D37" s="59" t="n">
@@ -2941,17 +2927,17 @@
         <f aca="false">PRODUCT(C37,D37)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="41"/>
-      <c r="B38" s="57" t="n">
+      <c r="A38" s="42"/>
+      <c r="B38" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A26</f>
         <v>1003</v>
       </c>
-      <c r="C38" s="58" t="n">
+      <c r="C38" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D38" s="59" t="n">
@@ -2970,17 +2956,17 @@
         <f aca="false">PRODUCT(C38,D38)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="41"/>
-      <c r="B39" s="57" t="n">
+      <c r="A39" s="42"/>
+      <c r="B39" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A27</f>
         <v>1004</v>
       </c>
-      <c r="C39" s="58" t="n">
+      <c r="C39" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D39" s="59" t="n">
@@ -2999,17 +2985,17 @@
         <f aca="false">PRODUCT(C39,D39)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="41"/>
-      <c r="B40" s="57" t="n">
+      <c r="A40" s="42"/>
+      <c r="B40" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A28</f>
         <v>0</v>
       </c>
-      <c r="C40" s="58" t="n">
+      <c r="C40" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D40" s="59" t="n">
@@ -3028,17 +3014,17 @@
         <f aca="false">PRODUCT(C40,D40)</f>
         <v>0</v>
       </c>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="41"/>
-      <c r="B41" s="57" t="n">
+      <c r="A41" s="42"/>
+      <c r="B41" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A29</f>
         <v>0</v>
       </c>
-      <c r="C41" s="58" t="n">
+      <c r="C41" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D41" s="59" t="n">
@@ -3057,17 +3043,17 @@
         <f aca="false">PRODUCT(C41,D41)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="41"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="41"/>
-      <c r="B42" s="57" t="n">
+      <c r="A42" s="42"/>
+      <c r="B42" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A30</f>
         <v>0</v>
       </c>
-      <c r="C42" s="58" t="n">
+      <c r="C42" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D42" s="59" t="n">
@@ -3086,17 +3072,17 @@
         <f aca="false">PRODUCT(C42,D42)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="41"/>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="41"/>
-      <c r="B43" s="57" t="n">
+      <c r="A43" s="42"/>
+      <c r="B43" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A31</f>
         <v>0</v>
       </c>
-      <c r="C43" s="58" t="n">
+      <c r="C43" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D43" s="59" t="n">
@@ -3115,17 +3101,17 @@
         <f aca="false">PRODUCT(C43,D43)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="41"/>
-      <c r="B44" s="57" t="n">
+      <c r="A44" s="42"/>
+      <c r="B44" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A32</f>
         <v>0</v>
       </c>
-      <c r="C44" s="58" t="n">
+      <c r="C44" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D44" s="59" t="n">
@@ -3144,17 +3130,17 @@
         <f aca="false">PRODUCT(C44,D44)</f>
         <v>0</v>
       </c>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="41"/>
-      <c r="B45" s="57" t="n">
+      <c r="A45" s="42"/>
+      <c r="B45" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A33</f>
         <v>0</v>
       </c>
-      <c r="C45" s="58" t="n">
+      <c r="C45" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D45" s="59" t="n">
@@ -3173,17 +3159,17 @@
         <f aca="false">PRODUCT(C45,D45)</f>
         <v>0</v>
       </c>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="41"/>
-      <c r="B46" s="57" t="n">
+      <c r="A46" s="42"/>
+      <c r="B46" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A34</f>
         <v>0</v>
       </c>
-      <c r="C46" s="58" t="n">
+      <c r="C46" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D46" s="59" t="n">
@@ -3202,17 +3188,17 @@
         <f aca="false">PRODUCT(C46,D46)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="41"/>
-      <c r="B47" s="57" t="n">
+      <c r="A47" s="42"/>
+      <c r="B47" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A35</f>
         <v>0</v>
       </c>
-      <c r="C47" s="58" t="n">
+      <c r="C47" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D47" s="59" t="n">
@@ -3231,17 +3217,17 @@
         <f aca="false">PRODUCT(C47,D47)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="41"/>
-      <c r="B48" s="57" t="n">
+      <c r="A48" s="42"/>
+      <c r="B48" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A36</f>
         <v>0</v>
       </c>
-      <c r="C48" s="58" t="n">
+      <c r="C48" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D48" s="59" t="n">
@@ -3260,17 +3246,17 @@
         <f aca="false">PRODUCT(C48,D48)</f>
         <v>0</v>
       </c>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="41"/>
-      <c r="B49" s="57" t="n">
+      <c r="A49" s="42"/>
+      <c r="B49" s="58" t="n">
         <f aca="false">'Pricing Transparency'!A37</f>
         <v>0</v>
       </c>
-      <c r="C49" s="58" t="n">
+      <c r="C49" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D49" s="59" t="n">
@@ -3289,16 +3275,17 @@
         <f aca="false">PRODUCT(C49,D49)</f>
         <v>0</v>
       </c>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H6"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3321,7 +3308,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="63" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="64" width="14.59"/>
@@ -3331,16 +3318,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3351,10 +3338,10 @@
         <v>100</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,10 +3352,10 @@
         <v>100</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3379,10 +3366,10 @@
         <v>100</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,10 +3380,10 @@
         <v>100</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,10 +3394,10 @@
         <v>100</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,10 +3408,10 @@
         <v>100</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,10 +3422,10 @@
         <v>100</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,10 +3436,10 @@
         <v>50</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3463,10 +3450,10 @@
         <v>100</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3477,10 +3464,10 @@
         <v>100</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3491,10 +3478,10 @@
         <v>100</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,10 +3492,10 @@
         <v>150</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3519,10 +3506,10 @@
         <v>300</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3533,10 +3520,10 @@
         <v>600</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3547,10 +3534,10 @@
         <v>450</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3561,10 +3548,10 @@
         <v>50</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,10 +3562,10 @@
         <v>100</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,10 +3576,10 @@
         <v>100</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3603,10 +3590,10 @@
         <v>200</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3617,10 +3604,10 @@
         <v>300</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3631,10 +3618,10 @@
         <v>50</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3645,10 +3632,10 @@
         <v>100</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3659,10 +3646,10 @@
         <v>100</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3673,10 +3660,10 @@
         <v>100</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3687,10 +3674,10 @@
         <v>100</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3701,10 +3688,10 @@
         <v>100</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pricing Transparency prices updates, invoice template added source
</commit_message>
<xml_diff>
--- a/MBP_Invoice_Template.xlsx
+++ b/MBP_Invoice_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Print" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
   <si>
     <t xml:space="preserve">Invoice</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/madebyparry/Freelance-Pricing-Project</t>
   </si>
   <si>
     <t xml:space="preserve">Subtotal</t>
@@ -293,7 +299,7 @@
     <numFmt numFmtId="171" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="172" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -377,6 +383,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FFC9211E"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Ubuntu Mono"/>
       <family val="3"/>
@@ -493,7 +520,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,7 +601,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -586,10 +613,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -610,12 +633,24 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -626,6 +661,10 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -670,7 +709,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -738,7 +777,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -855,7 +894,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -875,9 +914,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>544320</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1889280</xdr:rowOff>
+      <xdr:rowOff>1888920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -891,7 +930,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12600" y="210600"/>
-          <a:ext cx="7417800" cy="1678680"/>
+          <a:ext cx="7417440" cy="1678320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -912,9 +951,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>54720</xdr:colOff>
+      <xdr:colOff>54360</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>623520</xdr:rowOff>
+      <xdr:rowOff>623160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -928,7 +967,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5810760" y="8607600"/>
-          <a:ext cx="1129680" cy="529200"/>
+          <a:ext cx="1129320" cy="528840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -949,9 +988,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1306440</xdr:colOff>
+      <xdr:colOff>1306080</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -965,7 +1004,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1714320" y="7779600"/>
-          <a:ext cx="1433520" cy="603360"/>
+          <a:ext cx="1433160" cy="603000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -991,11 +1030,11 @@
   </sheetPr>
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.94"/>
@@ -1156,13 +1195,13 @@
         <f aca="false">Data!B16</f>
         <v>2</v>
       </c>
-      <c r="C10" s="23" t="str">
+      <c r="C10" s="20" t="str">
         <f aca="false">Data!E16</f>
-        <v>Basic Stack Setup </v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+        <v>Basic Stack Setup</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="21" t="n">
         <f aca="false">Data!D16</f>
         <v>150</v>
@@ -1214,13 +1253,13 @@
         <f aca="false">Data!B18</f>
         <v>4</v>
       </c>
-      <c r="C12" s="23" t="str">
+      <c r="C12" s="20" t="str">
         <f aca="false">Data!E18</f>
         <v>Event Booking System</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="21" t="n">
         <f aca="false">Data!D18</f>
         <v>350</v>
@@ -1301,13 +1340,13 @@
         <f aca="false">Data!B21</f>
         <v>7</v>
       </c>
-      <c r="C15" s="23" t="str">
+      <c r="C15" s="20" t="str">
         <f aca="false">Data!E21</f>
         <v>CDN Setup</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="21" t="n">
         <f aca="false">Data!D21</f>
         <v>100</v>
@@ -1388,13 +1427,13 @@
         <f aca="false">Data!B24</f>
         <v>11</v>
       </c>
-      <c r="C18" s="23" t="str">
+      <c r="C18" s="20" t="str">
         <f aca="false">Data!E24</f>
         <v>File Structuring &gt;500</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">Data!D24</f>
         <v>100</v>
@@ -1417,13 +1456,13 @@
         <f aca="false">Data!B25</f>
         <v>12</v>
       </c>
-      <c r="C19" s="23" t="str">
+      <c r="C19" s="20" t="str">
         <f aca="false">Data!E25</f>
         <v>File Sanitation</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="21" t="n">
         <f aca="false">Data!D25</f>
         <v>100</v>
@@ -1481,7 +1520,7 @@
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="23"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="21" t="n">
         <f aca="false">Data!D27</f>
         <v>100</v>
@@ -1504,13 +1543,13 @@
         <f aca="false">Data!B28</f>
         <v>21</v>
       </c>
-      <c r="C22" s="23" t="str">
+      <c r="C22" s="20" t="str">
         <f aca="false">Data!E28</f>
         <v>Static Pages</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="21" t="n">
         <f aca="false">Data!D28</f>
         <v>50</v>
@@ -1562,13 +1601,13 @@
         <f aca="false">Data!B30</f>
         <v>23</v>
       </c>
-      <c r="C24" s="23" t="str">
+      <c r="C24" s="20" t="str">
         <f aca="false">Data!E30</f>
         <v>Custom Feed</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="21" t="n">
         <f aca="false">Data!D30</f>
         <v>100</v>
@@ -1597,7 +1636,7 @@
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
-      <c r="F25" s="23"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="21" t="n">
         <f aca="false">Data!D31</f>
         <v>100</v>
@@ -1620,13 +1659,13 @@
         <f aca="false">Data!B32</f>
         <v>25</v>
       </c>
-      <c r="C26" s="23" t="str">
+      <c r="C26" s="20" t="str">
         <f aca="false">Data!E32</f>
         <v>Custom Backend Components</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="21" t="n">
         <f aca="false">Data!D32</f>
         <v>150</v>
@@ -1649,13 +1688,13 @@
         <f aca="false">Data!B33</f>
         <v>26</v>
       </c>
-      <c r="C27" s="23" t="str">
+      <c r="C27" s="20" t="str">
         <f aca="false">Data!E33</f>
         <v>Feed Architecture Setup</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="21" t="n">
         <f aca="false">Data!D33</f>
         <v>500</v>
@@ -1678,13 +1717,13 @@
         <f aca="false">Data!B34</f>
         <v>51</v>
       </c>
-      <c r="C28" s="23" t="str">
+      <c r="C28" s="20" t="str">
         <f aca="false">Data!E34</f>
         <v>Site Migration &gt;50 Pages</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="21" t="n">
         <f aca="false">Data!D34</f>
         <v>300</v>
@@ -1713,7 +1752,7 @@
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="23"/>
+      <c r="F29" s="20"/>
       <c r="G29" s="21" t="n">
         <f aca="false">Data!D35</f>
         <v>600</v>
@@ -1736,13 +1775,13 @@
         <f aca="false">Data!B36</f>
         <v>101</v>
       </c>
-      <c r="C30" s="23" t="str">
+      <c r="C30" s="20" t="str">
         <f aca="false">Data!E36</f>
         <v>Storefront – Woocommerce</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="21" t="n">
         <f aca="false">Data!D36</f>
         <v>450</v>
@@ -1765,13 +1804,13 @@
         <f aca="false">Data!B37</f>
         <v>500</v>
       </c>
-      <c r="C31" s="23" t="str">
+      <c r="C31" s="20" t="str">
         <f aca="false">Data!E37</f>
         <v>General Asset fixes</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="21" t="n">
         <f aca="false">Data!D37</f>
         <v>50</v>
@@ -1794,13 +1833,13 @@
         <f aca="false">Data!B38</f>
         <v>501</v>
       </c>
-      <c r="C32" s="23" t="str">
+      <c r="C32" s="20" t="str">
         <f aca="false">Data!E38</f>
         <v>Custom Illustration</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="21" t="n">
         <f aca="false">Data!D38</f>
         <v>100</v>
@@ -1823,13 +1862,13 @@
         <f aca="false">Data!B39</f>
         <v>502</v>
       </c>
-      <c r="C33" s="23" t="str">
+      <c r="C33" s="20" t="str">
         <f aca="false">Data!E39</f>
         <v>Custom Design Elements</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="21" t="n">
         <f aca="false">Data!D39</f>
         <v>100</v>
@@ -1852,13 +1891,13 @@
         <f aca="false">Data!B40</f>
         <v>503</v>
       </c>
-      <c r="C34" s="23" t="str">
+      <c r="C34" s="20" t="str">
         <f aca="false">Data!E40</f>
         <v>Logo Rework</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="21" t="n">
         <f aca="false">Data!D40</f>
         <v>200</v>
@@ -1881,13 +1920,13 @@
         <f aca="false">Data!B41</f>
         <v>504</v>
       </c>
-      <c r="C35" s="23" t="str">
+      <c r="C35" s="20" t="str">
         <f aca="false">Data!E41</f>
         <v>Brand Organization</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
       <c r="G35" s="21" t="n">
         <f aca="false">Data!D41</f>
         <v>300</v>
@@ -1910,13 +1949,13 @@
         <f aca="false">Data!B42</f>
         <v>505</v>
       </c>
-      <c r="C36" s="23" t="str">
+      <c r="C36" s="20" t="str">
         <f aca="false">Data!E42</f>
         <v>Copywriting</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="21" t="n">
         <f aca="false">Data!D42</f>
         <v>50</v>
@@ -1939,13 +1978,13 @@
         <f aca="false">Data!B43</f>
         <v>1000</v>
       </c>
-      <c r="C37" s="23" t="str">
+      <c r="C37" s="20" t="str">
         <f aca="false">Data!E43</f>
         <v>General Contracting</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="21" t="n">
         <f aca="false">Data!D43</f>
         <v>100</v>
@@ -1968,13 +2007,13 @@
         <f aca="false">Data!B44</f>
         <v>1001</v>
       </c>
-      <c r="C38" s="23" t="str">
+      <c r="C38" s="20" t="str">
         <f aca="false">Data!E44</f>
         <v>Web Consultation</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="21" t="n">
         <f aca="false">Data!D44</f>
         <v>100</v>
@@ -1997,13 +2036,13 @@
         <f aca="false">Data!B45</f>
         <v>1002</v>
       </c>
-      <c r="C39" s="23" t="str">
+      <c r="C39" s="20" t="str">
         <f aca="false">Data!E45</f>
         <v>Branding Consultation</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="21" t="n">
         <f aca="false">Data!D45</f>
         <v>100</v>
@@ -2026,13 +2065,13 @@
         <f aca="false">Data!B46</f>
         <v>1003</v>
       </c>
-      <c r="C40" s="23" t="str">
+      <c r="C40" s="20" t="str">
         <f aca="false">Data!E46</f>
         <v>Hosting Consultation</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="21" t="n">
         <f aca="false">Data!D46</f>
         <v>100</v>
@@ -2055,13 +2094,13 @@
         <f aca="false">Data!B47</f>
         <v>1004</v>
       </c>
-      <c r="C41" s="23" t="str">
+      <c r="C41" s="20" t="str">
         <f aca="false">Data!E47</f>
         <v>Sales Consultation</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="21" t="n">
         <f aca="false">Data!D47</f>
         <v>100</v>
@@ -2084,13 +2123,13 @@
         <f aca="false">Data!B48</f>
         <v>0</v>
       </c>
-      <c r="C42" s="23" t="n">
+      <c r="C42" s="20" t="n">
         <f aca="false">Data!E48</f>
         <v>0</v>
       </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="21" t="n">
         <f aca="false">Data!D48</f>
         <v>0</v>
@@ -2113,13 +2152,13 @@
         <f aca="false">Data!B49</f>
         <v>0</v>
       </c>
-      <c r="C43" s="23" t="n">
+      <c r="C43" s="20" t="n">
         <f aca="false">Data!E49</f>
         <v>0</v>
       </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
       <c r="G43" s="21" t="n">
         <f aca="false">Data!D49</f>
         <v>0</v>
@@ -2142,13 +2181,13 @@
         <f aca="false">Data!B50</f>
         <v>0</v>
       </c>
-      <c r="C44" s="23" t="n">
+      <c r="C44" s="20" t="n">
         <f aca="false">Data!E50</f>
         <v>0</v>
       </c>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="21" t="n">
         <f aca="false">Data!D50</f>
         <v>0</v>
@@ -2171,13 +2210,13 @@
         <f aca="false">Data!B51</f>
         <v>0</v>
       </c>
-      <c r="C45" s="23" t="n">
+      <c r="C45" s="20" t="n">
         <f aca="false">Data!E51</f>
         <v>0</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
       <c r="G45" s="21" t="n">
         <f aca="false">Data!D51</f>
         <v>0</v>
@@ -2200,13 +2239,13 @@
         <f aca="false">Data!B52</f>
         <v>0</v>
       </c>
-      <c r="C46" s="23" t="n">
+      <c r="C46" s="20" t="n">
         <f aca="false">Data!E52</f>
         <v>0</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
       <c r="G46" s="21" t="n">
         <f aca="false">Data!D52</f>
         <v>0</v>
@@ -2229,13 +2268,13 @@
         <f aca="false">Data!B53</f>
         <v>0</v>
       </c>
-      <c r="C47" s="23" t="n">
+      <c r="C47" s="20" t="n">
         <f aca="false">Data!E53</f>
         <v>0</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
       <c r="G47" s="21" t="n">
         <f aca="false">Data!D53</f>
         <v>0</v>
@@ -2254,87 +2293,91 @@
     </row>
     <row r="48" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="18"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="28"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="27"/>
       <c r="K48" s="18"/>
       <c r="L48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="7.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="18"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="29"/>
+      <c r="B49" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>10</v>
+      </c>
       <c r="D49" s="4"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="18"/>
       <c r="H49" s="30"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="28"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="27"/>
       <c r="K49" s="18"/>
       <c r="L49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="18"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="29"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="31"/>
       <c r="D50" s="4"/>
       <c r="E50" s="18"/>
       <c r="F50" s="18"/>
       <c r="G50" s="18"/>
-      <c r="H50" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="I50" s="32" t="n">
+      <c r="H50" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" s="34" t="n">
         <f aca="false">Data!F7</f>
         <v>2450</v>
       </c>
-      <c r="J50" s="28"/>
+      <c r="J50" s="27"/>
       <c r="K50" s="18"/>
       <c r="L50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="18"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="29"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="31"/>
       <c r="D51" s="4"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
       <c r="G51" s="18"/>
-      <c r="H51" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="I51" s="32" t="n">
+      <c r="H51" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="34" t="n">
         <f aca="false">Data!G4</f>
         <v>0</v>
       </c>
-      <c r="J51" s="28"/>
+      <c r="J51" s="27"/>
       <c r="K51" s="18"/>
       <c r="L51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="18"/>
-      <c r="B52" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" s="34"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
+      <c r="B52" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="37"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
       <c r="F52" s="18"/>
-      <c r="H52" s="33" t="s">
+      <c r="H52" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="32" t="n">
+      <c r="I52" s="34" t="n">
         <f aca="false">Data!G7</f>
         <v>2450</v>
       </c>
-      <c r="J52" s="36"/>
+      <c r="J52" s="39"/>
       <c r="K52" s="18"/>
       <c r="L52" s="4"/>
     </row>
@@ -2345,34 +2388,34 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="18"/>
-      <c r="H53" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53" s="32" t="n">
+      <c r="H53" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="34" t="n">
         <f aca="false">Data!F8</f>
         <v>0</v>
       </c>
-      <c r="J53" s="37"/>
+      <c r="J53" s="40"/>
       <c r="K53" s="18"/>
       <c r="L53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="18"/>
-      <c r="B54" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="38"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
+      <c r="B54" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="41"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="18"/>
-      <c r="H54" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="I54" s="32" t="n">
+      <c r="H54" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="34" t="n">
         <f aca="false">Data!F3</f>
         <v>0</v>
       </c>
-      <c r="J54" s="37"/>
+      <c r="J54" s="40"/>
       <c r="K54" s="18"/>
       <c r="L54" s="4"/>
     </row>
@@ -2382,15 +2425,15 @@
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
-      <c r="G55" s="34"/>
-      <c r="H55" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I55" s="40" t="n">
+      <c r="G55" s="37"/>
+      <c r="H55" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="I55" s="43" t="n">
         <f aca="false">Data!F10</f>
         <v>2450</v>
       </c>
-      <c r="J55" s="36"/>
+      <c r="J55" s="39"/>
       <c r="K55" s="18"/>
       <c r="L55" s="4"/>
     </row>
@@ -2429,7 +2472,7 @@
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="11"/>
-      <c r="F59" s="41"/>
+      <c r="F59" s="44"/>
       <c r="K59" s="10"/>
       <c r="L59" s="4"/>
     </row>
@@ -2449,7 +2492,7 @@
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="29"/>
+      <c r="F61" s="31"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
     </row>
@@ -2508,6 +2551,9 @@
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B54:C54"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C49" r:id="rId1" display="https://github.com/madebyparry/Freelance-Pricing-Project"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2515,7 +2561,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2543,1300 +2589,1300 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="44" t="s">
+      <c r="A3" s="45"/>
+      <c r="B3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="49"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
     </row>
     <row r="4" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="48" t="n">
+        <v>22</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="50"/>
+      <c r="E4" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="51" t="n">
         <f aca="false">IF(F5="Y",(PRODUCT(F7,0.5)+F4),F4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
     </row>
     <row r="5" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47"/>
-      <c r="B5" s="49" t="n">
+      <c r="A5" s="50"/>
+      <c r="B5" s="52" t="n">
         <v>45750</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="50" t="s">
+      <c r="C5" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
+      <c r="F5" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="54"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
     </row>
     <row r="6" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
     </row>
     <row r="7" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="53" t="n">
+      <c r="A7" s="50"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="56" t="n">
         <f aca="false">SUM(G15:G41)</f>
         <v>2450</v>
       </c>
-      <c r="G7" s="48" t="n">
+      <c r="G7" s="51" t="n">
         <f aca="false">IF(F5="Y",(PRODUCT(F7,0.5)-F4)-F3,F7-F4-F3)</f>
         <v>2450</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
     </row>
     <row r="8" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="53" t="n">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="56" t="n">
         <f aca="false">(G8*F6)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="54" t="n">
+      <c r="G8" s="57" t="n">
         <f aca="false">IF(F5="Y",(PRODUCT(F7,0.5)-F4),F7-F4)</f>
         <v>2450</v>
       </c>
-      <c r="H8" s="54"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
     </row>
     <row r="9" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47"/>
-      <c r="B9" s="55" t="n">
+      <c r="A9" s="50"/>
+      <c r="B9" s="58" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C9" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
+      <c r="C9" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
     </row>
     <row r="10" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="47"/>
-      <c r="B10" s="55" t="n">
+      <c r="A10" s="50"/>
+      <c r="B10" s="58" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="C10" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="44" t="s">
+      <c r="C10" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="57" t="n">
+      <c r="F10" s="60" t="n">
         <f aca="false">IF(F9="N",G7+F8,G7)</f>
         <v>2450</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="42"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="42"/>
-      <c r="B12" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="42"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="42"/>
-      <c r="B14" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="44" t="s">
+      <c r="A14" s="45"/>
+      <c r="B14" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="C14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="D14" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="E14" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
+      <c r="F14" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="42"/>
-      <c r="B15" s="58" t="n">
+      <c r="A15" s="45"/>
+      <c r="B15" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A2</f>
         <v>1</v>
       </c>
-      <c r="C15" s="52" t="n">
+      <c r="C15" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D15" s="59" t="n">
+      <c r="D15" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B2</f>
         <v>200</v>
       </c>
-      <c r="E15" s="60" t="str">
+      <c r="E15" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C2</f>
         <v>Website hosting – BASIC</v>
       </c>
-      <c r="F15" s="60" t="str">
+      <c r="F15" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D2</f>
         <v>/yr</v>
       </c>
-      <c r="G15" s="61" t="n">
+      <c r="G15" s="64" t="n">
         <f aca="false">PRODUCT(C15,D15)</f>
         <v>200</v>
       </c>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="42"/>
-      <c r="B16" s="58" t="n">
+      <c r="A16" s="45"/>
+      <c r="B16" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A3</f>
         <v>2</v>
       </c>
-      <c r="C16" s="52" t="n">
+      <c r="C16" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D16" s="59" t="n">
+      <c r="D16" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B3</f>
         <v>150</v>
       </c>
-      <c r="E16" s="60" t="str">
+      <c r="E16" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C3</f>
-        <v>Basic Stack Setup </v>
-      </c>
-      <c r="F16" s="60" t="str">
+        <v>Basic Stack Setup</v>
+      </c>
+      <c r="F16" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D3</f>
         <v>/site</v>
       </c>
-      <c r="G16" s="61" t="n">
+      <c r="G16" s="64" t="n">
         <f aca="false">PRODUCT(C16,D16)</f>
         <v>150</v>
       </c>
-      <c r="H16" s="62"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="42"/>
-      <c r="B17" s="58" t="n">
+      <c r="A17" s="45"/>
+      <c r="B17" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A4</f>
         <v>3</v>
       </c>
-      <c r="C17" s="52" t="n">
+      <c r="C17" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="59" t="n">
+      <c r="D17" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B4</f>
         <v>200</v>
       </c>
-      <c r="E17" s="60" t="str">
+      <c r="E17" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C4</f>
         <v>CMS Setup</v>
       </c>
-      <c r="F17" s="60" t="str">
+      <c r="F17" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D4</f>
         <v>/site</v>
       </c>
-      <c r="G17" s="61" t="n">
+      <c r="G17" s="64" t="n">
         <f aca="false">PRODUCT(C17,D17)</f>
         <v>200</v>
       </c>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42"/>
-      <c r="B18" s="58" t="n">
+      <c r="A18" s="45"/>
+      <c r="B18" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A5</f>
         <v>4</v>
       </c>
-      <c r="C18" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="59" t="n">
+      <c r="C18" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B5</f>
         <v>350</v>
       </c>
-      <c r="E18" s="60" t="str">
+      <c r="E18" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C5</f>
         <v>Event Booking System</v>
       </c>
-      <c r="F18" s="60" t="str">
+      <c r="F18" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D5</f>
         <v>/site</v>
       </c>
-      <c r="G18" s="61" t="n">
+      <c r="G18" s="64" t="n">
         <f aca="false">PRODUCT(C18,D18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42"/>
-      <c r="B19" s="58" t="n">
+      <c r="A19" s="45"/>
+      <c r="B19" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A6</f>
         <v>5</v>
       </c>
-      <c r="C19" s="52" t="n">
+      <c r="C19" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D19" s="59" t="n">
+      <c r="D19" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B6</f>
         <v>100</v>
       </c>
-      <c r="E19" s="60" t="str">
+      <c r="E19" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C6</f>
         <v>Domain Services</v>
       </c>
-      <c r="F19" s="60" t="str">
+      <c r="F19" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D6</f>
         <v>/domain</v>
       </c>
-      <c r="G19" s="61" t="n">
+      <c r="G19" s="64" t="n">
         <f aca="false">PRODUCT(C19,D19)</f>
         <v>100</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="42"/>
-      <c r="B20" s="58" t="n">
+      <c r="A20" s="45"/>
+      <c r="B20" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A7</f>
         <v>6</v>
       </c>
-      <c r="C20" s="52" t="n">
+      <c r="C20" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="59" t="n">
+      <c r="D20" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B7</f>
         <v>100</v>
       </c>
-      <c r="E20" s="60" t="str">
+      <c r="E20" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C7</f>
         <v>Email Setup</v>
       </c>
-      <c r="F20" s="60" t="str">
+      <c r="F20" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D7</f>
         <v>/network</v>
       </c>
-      <c r="G20" s="61" t="n">
+      <c r="G20" s="64" t="n">
         <f aca="false">PRODUCT(C20,D20)</f>
         <v>100</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42"/>
-      <c r="B21" s="58" t="n">
+      <c r="A21" s="45"/>
+      <c r="B21" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A8</f>
         <v>7</v>
       </c>
-      <c r="C21" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="59" t="n">
+      <c r="C21" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B8</f>
         <v>100</v>
       </c>
-      <c r="E21" s="60" t="str">
+      <c r="E21" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C8</f>
         <v>CDN Setup</v>
       </c>
-      <c r="F21" s="60" t="str">
+      <c r="F21" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D8</f>
         <v>/network</v>
       </c>
-      <c r="G21" s="61" t="n">
+      <c r="G21" s="64" t="n">
         <f aca="false">PRODUCT(C21,D21)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42"/>
-      <c r="B22" s="58" t="n">
+      <c r="A22" s="45"/>
+      <c r="B22" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A9</f>
         <v>8</v>
       </c>
-      <c r="C22" s="52" t="n">
+      <c r="C22" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D22" s="59" t="n">
+      <c r="D22" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B9</f>
         <v>150</v>
       </c>
-      <c r="E22" s="60" t="str">
+      <c r="E22" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C9</f>
         <v>Web Portal / Client Area</v>
       </c>
-      <c r="F22" s="60" t="str">
+      <c r="F22" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D9</f>
         <v>/site</v>
       </c>
-      <c r="G22" s="61" t="n">
+      <c r="G22" s="64" t="n">
         <f aca="false">PRODUCT(C22,D22)</f>
         <v>150</v>
       </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42"/>
-      <c r="B23" s="58" t="n">
+      <c r="A23" s="45"/>
+      <c r="B23" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A10</f>
         <v>9</v>
       </c>
-      <c r="C23" s="52" t="n">
+      <c r="C23" s="55" t="n">
         <v>1</v>
       </c>
-      <c r="D23" s="59" t="n">
+      <c r="D23" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B10</f>
         <v>350</v>
       </c>
-      <c r="E23" s="60" t="str">
+      <c r="E23" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C10</f>
         <v>Availability System</v>
       </c>
-      <c r="F23" s="60" t="str">
+      <c r="F23" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D10</f>
         <v>/site</v>
       </c>
-      <c r="G23" s="61" t="n">
+      <c r="G23" s="64" t="n">
         <f aca="false">PRODUCT(C23,D23)</f>
         <v>350</v>
       </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42"/>
-      <c r="B24" s="58" t="n">
+      <c r="A24" s="45"/>
+      <c r="B24" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A11</f>
         <v>11</v>
       </c>
-      <c r="C24" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="59" t="n">
+      <c r="C24" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B11</f>
         <v>100</v>
       </c>
-      <c r="E24" s="60" t="str">
+      <c r="E24" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C11</f>
         <v>File Structuring &gt;500</v>
       </c>
-      <c r="F24" s="60" t="str">
+      <c r="F24" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D11</f>
         <v>/dump</v>
       </c>
-      <c r="G24" s="61" t="n">
+      <c r="G24" s="64" t="n">
         <f aca="false">PRODUCT(C24,D24)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42"/>
-      <c r="B25" s="58" t="n">
+      <c r="A25" s="45"/>
+      <c r="B25" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A12</f>
         <v>12</v>
       </c>
-      <c r="C25" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="59" t="n">
+      <c r="C25" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B12</f>
         <v>100</v>
       </c>
-      <c r="E25" s="60" t="str">
+      <c r="E25" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C12</f>
         <v>File Sanitation</v>
       </c>
-      <c r="F25" s="60" t="str">
+      <c r="F25" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D12</f>
         <v>/dump</v>
       </c>
-      <c r="G25" s="61" t="n">
+      <c r="G25" s="64" t="n">
         <f aca="false">PRODUCT(C25,D25)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="45"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42"/>
-      <c r="B26" s="58" t="n">
+      <c r="A26" s="45"/>
+      <c r="B26" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A13</f>
         <v>13</v>
       </c>
-      <c r="C26" s="52" t="n">
+      <c r="C26" s="55" t="n">
         <v>4</v>
       </c>
-      <c r="D26" s="59" t="n">
+      <c r="D26" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B13</f>
         <v>100</v>
       </c>
-      <c r="E26" s="60" t="str">
+      <c r="E26" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C13</f>
         <v>Data Structuring</v>
       </c>
-      <c r="F26" s="60" t="str">
+      <c r="F26" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D13</f>
         <v>/hr</v>
       </c>
-      <c r="G26" s="61" t="n">
+      <c r="G26" s="64" t="n">
         <f aca="false">PRODUCT(C26,D26)</f>
         <v>400</v>
       </c>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="45"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42"/>
-      <c r="B27" s="58" t="n">
+      <c r="A27" s="45"/>
+      <c r="B27" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A14</f>
         <v>14</v>
       </c>
-      <c r="C27" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="59" t="n">
+      <c r="C27" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B14</f>
         <v>100</v>
       </c>
-      <c r="E27" s="60" t="str">
+      <c r="E27" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C14</f>
         <v>Content Organization</v>
       </c>
-      <c r="F27" s="60" t="str">
+      <c r="F27" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D14</f>
         <v>/hr</v>
       </c>
-      <c r="G27" s="61" t="n">
+      <c r="G27" s="64" t="n">
         <f aca="false">PRODUCT(C27,D27)</f>
         <v>0</v>
       </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="42"/>
-      <c r="B28" s="58" t="n">
+      <c r="A28" s="45"/>
+      <c r="B28" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A15</f>
         <v>21</v>
       </c>
-      <c r="C28" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="59" t="n">
+      <c r="C28" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B15</f>
         <v>50</v>
       </c>
-      <c r="E28" s="60" t="str">
+      <c r="E28" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C15</f>
         <v>Static Pages</v>
       </c>
-      <c r="F28" s="60" t="str">
+      <c r="F28" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D15</f>
         <v>/page</v>
       </c>
-      <c r="G28" s="61" t="n">
+      <c r="G28" s="64" t="n">
         <f aca="false">PRODUCT(C28,D28)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42"/>
-      <c r="B29" s="58" t="n">
+      <c r="A29" s="45"/>
+      <c r="B29" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A16</f>
         <v>22</v>
       </c>
-      <c r="C29" s="52" t="n">
+      <c r="C29" s="55" t="n">
         <v>8</v>
       </c>
-      <c r="D29" s="59" t="n">
+      <c r="D29" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B16</f>
         <v>100</v>
       </c>
-      <c r="E29" s="60" t="str">
+      <c r="E29" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C16</f>
         <v>Dynamic Pages</v>
       </c>
-      <c r="F29" s="60" t="str">
+      <c r="F29" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D16</f>
         <v>/page</v>
       </c>
-      <c r="G29" s="61" t="n">
+      <c r="G29" s="64" t="n">
         <f aca="false">PRODUCT(C29,D29)</f>
         <v>800</v>
       </c>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="42"/>
-      <c r="B30" s="58" t="n">
+      <c r="A30" s="45"/>
+      <c r="B30" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A17</f>
         <v>23</v>
       </c>
-      <c r="C30" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="59" t="n">
+      <c r="C30" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B17</f>
         <v>100</v>
       </c>
-      <c r="E30" s="60" t="str">
+      <c r="E30" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C17</f>
         <v>Custom Feed</v>
       </c>
-      <c r="F30" s="60" t="str">
+      <c r="F30" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D17</f>
         <v>/feed</v>
       </c>
-      <c r="G30" s="61" t="n">
+      <c r="G30" s="64" t="n">
         <f aca="false">PRODUCT(C30,D30)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42"/>
-      <c r="B31" s="58" t="n">
+      <c r="A31" s="45"/>
+      <c r="B31" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A18</f>
         <v>24</v>
       </c>
-      <c r="C31" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="59" t="n">
+      <c r="C31" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B18</f>
         <v>100</v>
       </c>
-      <c r="E31" s="60" t="str">
+      <c r="E31" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C18</f>
         <v>Custom Frontend Components</v>
       </c>
-      <c r="F31" s="60" t="str">
+      <c r="F31" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D18</f>
         <v>/component</v>
       </c>
-      <c r="G31" s="61" t="n">
+      <c r="G31" s="64" t="n">
         <f aca="false">PRODUCT(C31,D31)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="42"/>
-      <c r="B32" s="58" t="n">
+      <c r="A32" s="45"/>
+      <c r="B32" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A19</f>
         <v>25</v>
       </c>
-      <c r="C32" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="59" t="n">
+      <c r="C32" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B19</f>
         <v>150</v>
       </c>
-      <c r="E32" s="60" t="str">
+      <c r="E32" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C19</f>
         <v>Custom Backend Components</v>
       </c>
-      <c r="F32" s="60" t="str">
+      <c r="F32" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D19</f>
         <v>/component</v>
       </c>
-      <c r="G32" s="61" t="n">
+      <c r="G32" s="64" t="n">
         <f aca="false">PRODUCT(C32,D32)</f>
         <v>0</v>
       </c>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="42"/>
-      <c r="B33" s="58" t="n">
+      <c r="A33" s="45"/>
+      <c r="B33" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A20</f>
         <v>26</v>
       </c>
-      <c r="C33" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" s="59" t="n">
+      <c r="C33" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B20</f>
         <v>500</v>
       </c>
-      <c r="E33" s="60" t="str">
+      <c r="E33" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C20</f>
         <v>Feed Architecture Setup</v>
       </c>
-      <c r="F33" s="60" t="str">
+      <c r="F33" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D20</f>
         <v>/feed</v>
       </c>
-      <c r="G33" s="61" t="n">
+      <c r="G33" s="64" t="n">
         <f aca="false">PRODUCT(C33,D33)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="42"/>
-      <c r="B34" s="58" t="n">
+      <c r="A34" s="45"/>
+      <c r="B34" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A21</f>
         <v>51</v>
       </c>
-      <c r="C34" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="59" t="n">
+      <c r="C34" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B21</f>
         <v>300</v>
       </c>
-      <c r="E34" s="60" t="str">
+      <c r="E34" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C21</f>
         <v>Site Migration &gt;50 Pages</v>
       </c>
-      <c r="F34" s="60" t="str">
+      <c r="F34" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D21</f>
         <v>/site</v>
       </c>
-      <c r="G34" s="61" t="n">
+      <c r="G34" s="64" t="n">
         <f aca="false">PRODUCT(C34,D34)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="42"/>
-      <c r="B35" s="58" t="n">
+      <c r="A35" s="45"/>
+      <c r="B35" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A22</f>
         <v>52</v>
       </c>
-      <c r="C35" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" s="59" t="n">
+      <c r="C35" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B22</f>
         <v>600</v>
       </c>
-      <c r="E35" s="60" t="str">
+      <c r="E35" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C22</f>
         <v>Site Migration &gt;100&lt;50 Pages</v>
       </c>
-      <c r="F35" s="60" t="str">
+      <c r="F35" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D22</f>
         <v>/site</v>
       </c>
-      <c r="G35" s="61" t="n">
+      <c r="G35" s="64" t="n">
         <f aca="false">PRODUCT(C35,D35)</f>
         <v>0</v>
       </c>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="42"/>
-      <c r="B36" s="58" t="n">
+      <c r="A36" s="45"/>
+      <c r="B36" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A23</f>
         <v>101</v>
       </c>
-      <c r="C36" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" s="59" t="n">
+      <c r="C36" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B23</f>
         <v>450</v>
       </c>
-      <c r="E36" s="60" t="str">
+      <c r="E36" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C23</f>
         <v>Storefront – Woocommerce</v>
       </c>
-      <c r="F36" s="60" t="str">
+      <c r="F36" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D23</f>
         <v>/site</v>
       </c>
-      <c r="G36" s="61" t="n">
+      <c r="G36" s="64" t="n">
         <f aca="false">PRODUCT(C36,D36)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="42"/>
-      <c r="B37" s="58" t="n">
+      <c r="A37" s="45"/>
+      <c r="B37" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A24</f>
         <v>500</v>
       </c>
-      <c r="C37" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" s="59" t="n">
+      <c r="C37" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B24</f>
         <v>50</v>
       </c>
-      <c r="E37" s="60" t="str">
+      <c r="E37" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C24</f>
         <v>General Asset fixes</v>
       </c>
-      <c r="F37" s="60" t="str">
+      <c r="F37" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D24</f>
         <v>/asset</v>
       </c>
-      <c r="G37" s="61" t="n">
+      <c r="G37" s="64" t="n">
         <f aca="false">PRODUCT(C37,D37)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="42"/>
-      <c r="B38" s="58" t="n">
+      <c r="A38" s="45"/>
+      <c r="B38" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A25</f>
         <v>501</v>
       </c>
-      <c r="C38" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="59" t="n">
+      <c r="C38" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B25</f>
         <v>100</v>
       </c>
-      <c r="E38" s="60" t="str">
+      <c r="E38" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C25</f>
         <v>Custom Illustration</v>
       </c>
-      <c r="F38" s="60" t="str">
+      <c r="F38" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D25</f>
         <v>/hr</v>
       </c>
-      <c r="G38" s="61" t="n">
+      <c r="G38" s="64" t="n">
         <f aca="false">PRODUCT(C38,D38)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="42"/>
-      <c r="B39" s="58" t="n">
+      <c r="A39" s="45"/>
+      <c r="B39" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A26</f>
         <v>502</v>
       </c>
-      <c r="C39" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="59" t="n">
+      <c r="C39" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B26</f>
         <v>100</v>
       </c>
-      <c r="E39" s="60" t="str">
+      <c r="E39" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C26</f>
         <v>Custom Design Elements</v>
       </c>
-      <c r="F39" s="60" t="str">
+      <c r="F39" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D26</f>
         <v>/hr</v>
       </c>
-      <c r="G39" s="61" t="n">
+      <c r="G39" s="64" t="n">
         <f aca="false">PRODUCT(C39,D39)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="42"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="42"/>
-      <c r="B40" s="58" t="n">
+      <c r="A40" s="45"/>
+      <c r="B40" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A27</f>
         <v>503</v>
       </c>
-      <c r="C40" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" s="59" t="n">
+      <c r="C40" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B27</f>
         <v>200</v>
       </c>
-      <c r="E40" s="60" t="str">
+      <c r="E40" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C27</f>
         <v>Logo Rework</v>
       </c>
-      <c r="F40" s="60" t="str">
+      <c r="F40" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D27</f>
         <v>/item</v>
       </c>
-      <c r="G40" s="61" t="n">
+      <c r="G40" s="64" t="n">
         <f aca="false">PRODUCT(C40,D40)</f>
         <v>0</v>
       </c>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="45"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="42"/>
-      <c r="B41" s="58" t="n">
+      <c r="A41" s="45"/>
+      <c r="B41" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A28</f>
         <v>504</v>
       </c>
-      <c r="C41" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="59" t="n">
+      <c r="C41" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B28</f>
         <v>300</v>
       </c>
-      <c r="E41" s="60" t="str">
+      <c r="E41" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C28</f>
         <v>Brand Organization</v>
       </c>
-      <c r="F41" s="60" t="str">
+      <c r="F41" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D28</f>
         <v>/book</v>
       </c>
-      <c r="G41" s="61" t="n">
+      <c r="G41" s="64" t="n">
         <f aca="false">PRODUCT(C41,D41)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="45"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="42"/>
-      <c r="B42" s="58" t="n">
+      <c r="A42" s="45"/>
+      <c r="B42" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A29</f>
         <v>505</v>
       </c>
-      <c r="C42" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="59" t="n">
+      <c r="C42" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B29</f>
         <v>50</v>
       </c>
-      <c r="E42" s="60" t="str">
+      <c r="E42" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C29</f>
         <v>Copywriting</v>
       </c>
-      <c r="F42" s="60" t="str">
+      <c r="F42" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D29</f>
         <v>/item</v>
       </c>
-      <c r="G42" s="61" t="n">
+      <c r="G42" s="64" t="n">
         <f aca="false">PRODUCT(C42,D42)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="45"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="42"/>
-      <c r="B43" s="58" t="n">
+      <c r="A43" s="45"/>
+      <c r="B43" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A30</f>
         <v>1000</v>
       </c>
-      <c r="C43" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="59" t="n">
+      <c r="C43" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B30</f>
         <v>100</v>
       </c>
-      <c r="E43" s="60" t="str">
+      <c r="E43" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C30</f>
         <v>General Contracting</v>
       </c>
-      <c r="F43" s="60" t="str">
+      <c r="F43" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D30</f>
         <v>/30min</v>
       </c>
-      <c r="G43" s="61" t="n">
+      <c r="G43" s="64" t="n">
         <f aca="false">PRODUCT(C43,D43)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="45"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="42"/>
-      <c r="B44" s="58" t="n">
+      <c r="A44" s="45"/>
+      <c r="B44" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A31</f>
         <v>1001</v>
       </c>
-      <c r="C44" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="59" t="n">
+      <c r="C44" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B31</f>
         <v>100</v>
       </c>
-      <c r="E44" s="60" t="str">
+      <c r="E44" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C31</f>
         <v>Web Consultation</v>
       </c>
-      <c r="F44" s="60" t="str">
+      <c r="F44" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D31</f>
         <v>/30min</v>
       </c>
-      <c r="G44" s="61" t="n">
+      <c r="G44" s="64" t="n">
         <f aca="false">PRODUCT(C44,D44)</f>
         <v>0</v>
       </c>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="42"/>
-      <c r="B45" s="58" t="n">
+      <c r="A45" s="45"/>
+      <c r="B45" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A32</f>
         <v>1002</v>
       </c>
-      <c r="C45" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="59" t="n">
+      <c r="C45" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B32</f>
         <v>100</v>
       </c>
-      <c r="E45" s="60" t="str">
+      <c r="E45" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C32</f>
         <v>Branding Consultation</v>
       </c>
-      <c r="F45" s="60" t="str">
+      <c r="F45" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D32</f>
         <v>/30min</v>
       </c>
-      <c r="G45" s="61" t="n">
+      <c r="G45" s="64" t="n">
         <f aca="false">PRODUCT(C45,D45)</f>
         <v>0</v>
       </c>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="42"/>
-      <c r="B46" s="58" t="n">
+      <c r="A46" s="45"/>
+      <c r="B46" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A33</f>
         <v>1003</v>
       </c>
-      <c r="C46" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" s="59" t="n">
+      <c r="C46" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B33</f>
         <v>100</v>
       </c>
-      <c r="E46" s="60" t="str">
+      <c r="E46" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C33</f>
         <v>Hosting Consultation</v>
       </c>
-      <c r="F46" s="60" t="str">
+      <c r="F46" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D33</f>
         <v>/30min</v>
       </c>
-      <c r="G46" s="61" t="n">
+      <c r="G46" s="64" t="n">
         <f aca="false">PRODUCT(C46,D46)</f>
         <v>0</v>
       </c>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="45"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="42"/>
-      <c r="B47" s="58" t="n">
+      <c r="A47" s="45"/>
+      <c r="B47" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A34</f>
         <v>1004</v>
       </c>
-      <c r="C47" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="59" t="n">
+      <c r="C47" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B34</f>
         <v>100</v>
       </c>
-      <c r="E47" s="60" t="str">
+      <c r="E47" s="63" t="str">
         <f aca="false">'Pricing Transparency'!C34</f>
         <v>Sales Consultation</v>
       </c>
-      <c r="F47" s="60" t="str">
+      <c r="F47" s="63" t="str">
         <f aca="false">'Pricing Transparency'!D34</f>
         <v>/30min</v>
       </c>
-      <c r="G47" s="61" t="n">
+      <c r="G47" s="64" t="n">
         <f aca="false">PRODUCT(C47,D47)</f>
         <v>0</v>
       </c>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="45"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="42"/>
-      <c r="B48" s="58" t="n">
+      <c r="A48" s="45"/>
+      <c r="B48" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A35</f>
         <v>0</v>
       </c>
-      <c r="C48" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" s="59" t="n">
+      <c r="C48" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B35</f>
         <v>0</v>
       </c>
-      <c r="E48" s="60" t="n">
+      <c r="E48" s="63" t="n">
         <f aca="false">'Pricing Transparency'!C35</f>
         <v>0</v>
       </c>
-      <c r="F48" s="60" t="n">
+      <c r="F48" s="63" t="n">
         <f aca="false">'Pricing Transparency'!D35</f>
         <v>0</v>
       </c>
-      <c r="G48" s="61" t="n">
+      <c r="G48" s="64" t="n">
         <f aca="false">PRODUCT(C48,D48)</f>
         <v>0</v>
       </c>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="42"/>
-      <c r="B49" s="58" t="n">
+      <c r="A49" s="45"/>
+      <c r="B49" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A36</f>
         <v>0</v>
       </c>
-      <c r="C49" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="59" t="n">
+      <c r="C49" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B36</f>
         <v>0</v>
       </c>
-      <c r="E49" s="60" t="n">
+      <c r="E49" s="63" t="n">
         <f aca="false">'Pricing Transparency'!C36</f>
         <v>0</v>
       </c>
-      <c r="F49" s="60" t="n">
+      <c r="F49" s="63" t="n">
         <f aca="false">'Pricing Transparency'!D36</f>
         <v>0</v>
       </c>
-      <c r="G49" s="61" t="n">
+      <c r="G49" s="64" t="n">
         <f aca="false">PRODUCT(C49,D49)</f>
         <v>0</v>
       </c>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="42"/>
-      <c r="B50" s="58" t="n">
+      <c r="A50" s="45"/>
+      <c r="B50" s="61" t="n">
         <f aca="false">'Pricing Transparency'!A37</f>
         <v>0</v>
       </c>
-      <c r="C50" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="59" t="n">
+      <c r="C50" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="62" t="n">
         <f aca="false">'Pricing Transparency'!B37</f>
         <v>0</v>
       </c>
-      <c r="E50" s="60" t="n">
+      <c r="E50" s="63" t="n">
         <f aca="false">'Pricing Transparency'!C37</f>
         <v>0</v>
       </c>
-      <c r="F50" s="60" t="n">
+      <c r="F50" s="63" t="n">
         <f aca="false">'Pricing Transparency'!D37</f>
         <v>0</v>
       </c>
-      <c r="G50" s="61" t="n">
+      <c r="G50" s="64" t="n">
         <f aca="false">PRODUCT(C50,D50)</f>
         <v>0</v>
       </c>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
     </row>
   </sheetData>
   <autoFilter ref="B14:G50"/>
@@ -3865,16 +3911,16 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="63" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="64" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="64" width="35.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="64" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="66" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="67" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="67" width="35.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="67" width="18.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3882,13 +3928,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3899,10 +3945,10 @@
         <v>200</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3913,10 +3959,10 @@
         <v>150</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,10 +3973,10 @@
         <v>200</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3941,10 +3987,10 @@
         <v>350</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,10 +4001,10 @@
         <v>100</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3969,10 +4015,10 @@
         <v>100</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,10 +4029,10 @@
         <v>100</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3997,10 +4043,10 @@
         <v>150</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4011,10 +4057,10 @@
         <v>350</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4025,10 +4071,10 @@
         <v>100</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4039,10 +4085,10 @@
         <v>100</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4053,10 +4099,10 @@
         <v>100</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4067,10 +4113,10 @@
         <v>100</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4081,10 +4127,10 @@
         <v>50</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4095,10 +4141,10 @@
         <v>100</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4109,10 +4155,10 @@
         <v>100</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4123,10 +4169,10 @@
         <v>100</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4137,10 +4183,10 @@
         <v>150</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4151,10 +4197,10 @@
         <v>500</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,10 +4211,10 @@
         <v>300</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4179,10 +4225,10 @@
         <v>600</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4193,10 +4239,10 @@
         <v>450</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4207,10 +4253,10 @@
         <v>50</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4221,10 +4267,10 @@
         <v>100</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4235,10 +4281,10 @@
         <v>100</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,10 +4295,10 @@
         <v>200</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4263,10 +4309,10 @@
         <v>300</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4277,10 +4323,10 @@
         <v>50</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4291,10 +4337,10 @@
         <v>100</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4305,10 +4351,10 @@
         <v>100</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4319,10 +4365,10 @@
         <v>100</v>
       </c>
       <c r="C32" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4333,10 +4379,10 @@
         <v>100</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4347,10 +4393,10 @@
         <v>100</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>